<commit_message>
project update to jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/SignIn.xlsx
+++ b/src/test/resources/exceldata/SignIn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Roops/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uthik\git\DS_AlgoVer1\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FEFB36-7F44-4F4C-A965-1E2D4DD0BBC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD1845D-63C2-4747-93B5-003EA6649B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,20 +404,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="34.5" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,16 +426,16 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -444,7 +444,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -453,21 +453,25 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{4F202747-E251-4EFD-9F4E-742D63B5CC62}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{6BB9EAF7-D3CB-3D4E-9446-86A762665C4D}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{3CB85D80-4345-7E4F-94B1-FD9F2757705B}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{B584DDD0-371F-C343-B2B2-979B4E3171F8}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{3CB85D80-4345-7E4F-94B1-FD9F2757705B}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{E86BDBAE-383A-466C-B12B-E9F6D5D85B3D}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{44835D98-D098-47D8-9CA2-CE29E0EADD0A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>